<commit_message>
Integrated new order and schedule
Manually entry of new order and schedule is integrated and functional

Excel import:
1. Create Order and scheduling integrated and functional
2. Return page with List of errors and successful insert.
</commit_message>
<xml_diff>
--- a/Content/sampleExcel.xlsx
+++ b/Content/sampleExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Venture Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{91950F8C-4CA8-4B4C-AA95-D5F04FB747C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADE7AFAC-265B-440C-BAF1-566971330A00}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{91950F8C-4CA8-4B4C-AA95-D5F04FB747C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9CEF6F37-0539-4494-A298-8EA8CE738191}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="1943" windowWidth="10268" windowHeight="9465" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
+    <workbookView xWindow="4305" yWindow="1927" windowWidth="13778" windowHeight="9466" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>orderId</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Venture Order List</t>
+  </si>
+  <si>
+    <t>test excel 2</t>
+  </si>
+  <si>
+    <t>1/12/2019  12:12PM</t>
   </si>
 </sst>
 </file>
@@ -422,15 +428,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C943A-3D35-41B8-B784-28D36878AB63}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.59765625" customWidth="1"/>
+    <col min="5" max="5" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -473,11 +480,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
-        <v>43800</v>
-      </c>
-      <c r="E3" s="1">
-        <v>43833</v>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F3">
         <v>999</v>
@@ -490,11 +497,11 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
-        <v>43800</v>
-      </c>
-      <c r="E4" s="1">
-        <v>43833</v>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F4">
         <v>999</v>
@@ -510,13 +517,33 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
-        <v>43800</v>
-      </c>
-      <c r="E5" s="1">
-        <v>43833</v>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F5">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
         <v>999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug fixes and changes to edit orders
Added 2 new columns in Orders table
- status (refers to status of orders)
-priority (range from 1(highest)-3(lowest))

made changes to controller and view to add option to change status and priority of orders
</commit_message>
<xml_diff>
--- a/Content/sampleExcel.xlsx
+++ b/Content/sampleExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Venture Scheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{91950F8C-4CA8-4B4C-AA95-D5F04FB747C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9CEF6F37-0539-4494-A298-8EA8CE738191}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D64AC-35D5-4AD2-986D-49065CE63DCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="1927" windowWidth="13778" windowHeight="9466" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
+    <workbookView xWindow="1485" yWindow="1657" windowWidth="18840" windowHeight="9466" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,10 @@
     <t>Venture Order List</t>
   </si>
   <si>
-    <t>test excel 2</t>
-  </si>
-  <si>
     <t>1/12/2019  12:12PM</t>
+  </si>
+  <si>
+    <t>test review</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -481,10 +481,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>999</v>
@@ -498,10 +498,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>999</v>
@@ -518,10 +518,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>999</v>
@@ -529,22 +529,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>20</v>
+        <v>9874</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>999</v>
+        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a review page for Orders(reviewOrderCSVPost)
1. enable users to view excel orders import.
2. enable user to make changes
3. enable users to select which orders they do not want schedule
</commit_message>
<xml_diff>
--- a/Content/sampleExcel.xlsx
+++ b/Content/sampleExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D64AC-35D5-4AD2-986D-49065CE63DCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9FE745-FEA3-4950-BB59-B50EBCF4C649}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="1657" windowWidth="18840" windowHeight="9466" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
   </bookViews>
@@ -529,7 +529,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>9874</v>
+        <v>9873</v>
       </c>
       <c r="B6">
         <v>5</v>

</xml_diff>

<commit_message>
Review orders CSV page
-allows user to review and make changes to orders that are imported via CSV.
-allows users to select and choose orders to schedule.
-schedule selected CSV orders based on shipping date priority
</commit_message>
<xml_diff>
--- a/Content/sampleExcel.xlsx
+++ b/Content/sampleExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9FE745-FEA3-4950-BB59-B50EBCF4C649}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0DDC36-BD26-4BF5-8152-DED7FB8466FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="1657" windowWidth="18840" windowHeight="9466" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
+    <workbookView xWindow="525" yWindow="3225" windowWidth="19260" windowHeight="9855" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,36 +31,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>orderId</t>
   </si>
   <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>lastMaterialDate</t>
+  </si>
+  <si>
+    <t>shipDate</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Venture Order List</t>
+  </si>
+  <si>
+    <t>Test order 1</t>
+  </si>
+  <si>
+    <t>Test order 2</t>
+  </si>
+  <si>
+    <t>Test order 3</t>
+  </si>
+  <si>
+    <t>Test order 4</t>
+  </si>
+  <si>
+    <t>1/1/2020  12:00PM</t>
+  </si>
+  <si>
+    <t>12/3/2020  12:00PM</t>
+  </si>
+  <si>
+    <t>15/4/2020  12:00PM</t>
+  </si>
+  <si>
+    <t>30/03/2020  12:00PM</t>
+  </si>
+  <si>
+    <t>16/12/2020  12:12PM</t>
+  </si>
+  <si>
+    <t>30/4/2020  12:12PM</t>
+  </si>
+  <si>
     <t>partId</t>
   </si>
   <si>
-    <t>projectName</t>
-  </si>
-  <si>
-    <t>lastMaterialDate</t>
-  </si>
-  <si>
-    <t>shipDate</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>test excel inport</t>
-  </si>
-  <si>
-    <t>Venture Order List</t>
-  </si>
-  <si>
-    <t>1/12/2019  12:12PM</t>
-  </si>
-  <si>
-    <t>test review</t>
+    <t>30/3/2020  12:00PM</t>
   </si>
 </sst>
 </file>
@@ -431,7 +455,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -442,7 +466,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -455,36 +479,36 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3003</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>999</v>
@@ -494,14 +518,17 @@
       <c r="A4">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" s="2">
+        <v>3007</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>999</v>
@@ -509,19 +536,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3008</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>999</v>
@@ -529,22 +556,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>9873</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3008</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>1234</v>
+        <v>999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated scheduling algo and operator start/stop process
1. if backend process does not have exist for part. one is automatically created by system with backend time = 0.

2. update scheduling algorithm when (reviewOrderCSVSchedule) to sort orders based on lastMaterialDate then by shipdate

3. added smtStart and Stop process.

4. integrated ganttchart display.
</commit_message>
<xml_diff>
--- a/Content/sampleExcel.xlsx
+++ b/Content/sampleExcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E73EFD-337B-4E23-AD7A-69DC16E48684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C41BE8-9C1B-41D9-B4B6-E60EA91DA9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1013" yWindow="1283" windowWidth="19260" windowHeight="9855" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
   </bookViews>

</xml_diff>

<commit_message>
Updates to View schedule
1. completed testing on the schedule filtering of status and lines.

2.	Changes to view schedule
a.	Added the order status to schedule table
b.	Added status filter
c.	Added line filter

3. changed color team to white and grey theme

4. Added row highlight red when order is late for shipping
</commit_message>
<xml_diff>
--- a/Content/sampleExcel.xlsx
+++ b/Content/sampleExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D700D4-311C-4C9A-A036-22FBADE9A2AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9992ACE-55C7-4169-BBFD-95F780938ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1013" yWindow="1283" windowWidth="19260" windowHeight="9855" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
+    <workbookView xWindow="1020" yWindow="1290" windowWidth="19260" windowHeight="9855" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>orderId</t>
   </si>
@@ -75,16 +75,37 @@
     <t>30/3/2020  12:00PM</t>
   </si>
   <si>
-    <t>Work order 1</t>
-  </si>
-  <si>
-    <t>Work order 2</t>
-  </si>
-  <si>
-    <t>Work order 3</t>
-  </si>
-  <si>
-    <t>Work order 4</t>
+    <t>6/2/2020  12:00PM</t>
+  </si>
+  <si>
+    <t>06/06/2020 12:00PM</t>
+  </si>
+  <si>
+    <t>10/07/2020 12:00PM</t>
+  </si>
+  <si>
+    <t>08/08/2020 12:00PM</t>
+  </si>
+  <si>
+    <t>Work order 21</t>
+  </si>
+  <si>
+    <t>Work order 22</t>
+  </si>
+  <si>
+    <t>Work order 23</t>
+  </si>
+  <si>
+    <t>Work order 24</t>
+  </si>
+  <si>
+    <t>work order 25</t>
+  </si>
+  <si>
+    <t>work order 26</t>
+  </si>
+  <si>
+    <t>work order 27</t>
   </si>
 </sst>
 </file>
@@ -453,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C943A-3D35-41B8-B784-28D36878AB63}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -498,13 +519,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -518,13 +539,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -538,13 +559,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -558,13 +579,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -574,6 +595,66 @@
       </c>
       <c r="F6">
         <v>999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>9520</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>5460</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>7800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
View orders delete confimation
Added sweet alert for user confimation before deleteing orders
</commit_message>
<xml_diff>
--- a/Content/sampleExcel.xlsx
+++ b/Content/sampleExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F485C2-C91A-4ABE-9C8A-6E150B5B571F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E64F101-0074-47D9-8EC1-AAE2BFED223F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7935" yWindow="1425" windowWidth="10770" windowHeight="9450" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
+    <workbookView xWindow="375" yWindow="435" windowWidth="18330" windowHeight="10440" xr2:uid="{FFE1BEEC-108B-44F3-AF2B-7D255C43225C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>orderId</t>
   </si>
@@ -115,13 +115,46 @@
   </si>
   <si>
     <t>05/05/2020 12:00PM</t>
+  </si>
+  <si>
+    <t>work order 29</t>
+  </si>
+  <si>
+    <t>work order 30</t>
+  </si>
+  <si>
+    <t>work order 31</t>
+  </si>
+  <si>
+    <t>work order 32</t>
+  </si>
+  <si>
+    <t>work order 33</t>
+  </si>
+  <si>
+    <t>work order 34</t>
+  </si>
+  <si>
+    <t>work order 35</t>
+  </si>
+  <si>
+    <t>work order 36</t>
+  </si>
+  <si>
+    <t>18/03/2020 12:00PM</t>
+  </si>
+  <si>
+    <t>10/06/2020 12:00PM</t>
+  </si>
+  <si>
+    <t>30/03/2020 12:00PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +166,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -483,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C943A-3D35-41B8-B784-28D36878AB63}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -683,13 +722,174 @@
         <v>27</v>
       </c>
       <c r="F10">
-        <v>500</v>
+        <v>2652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12">
+        <v>9583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16">
+        <v>3572</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>2892</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>5652</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>